<commit_message>
Added features for demo
</commit_message>
<xml_diff>
--- a/data/Wits Staff Bursary(1).xlsx
+++ b/data/Wits Staff Bursary(1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tumelo Maphalla\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5614A1-8223-4AE5-A227-0FC3C329BF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696D3097-D0A3-495D-8C3B-76718ECCED8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{26B25BEA-3BCE-40F4-888B-FAB2E5F6A6A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>Username</t>
   </si>
@@ -180,13 +180,58 @@
   </si>
   <si>
     <t>Full_PartTime</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>msedge.exe</t>
+  </si>
+  <si>
+    <t>https://qa.intranetapps.wits.ac.za/was/applogin</t>
+  </si>
+  <si>
+    <t>A0090655</t>
+  </si>
+  <si>
+    <t>LineManagerUsername</t>
+  </si>
+  <si>
+    <t>HRApprover</t>
+  </si>
+  <si>
+    <t>HRUsername</t>
+  </si>
+  <si>
+    <t>UploadedFilePathTxt</t>
+  </si>
+  <si>
+    <t>UploadedFilePathDocx</t>
+  </si>
+  <si>
+    <t>A0031536</t>
+  </si>
+  <si>
+    <t>Keitha January</t>
+  </si>
+  <si>
+    <t>A0026159</t>
+  </si>
+  <si>
+    <t>\data\empty_file.txt</t>
+  </si>
+  <si>
+    <t>\data\empty_file.docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +249,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -229,10 +280,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A375A088-B849-4403-87DE-33B0A5ACC6B2}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,7 +642,7 @@
     <col min="21" max="21" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,8 +721,29 @@
       <c r="Z1" t="s">
         <v>47</v>
       </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -749,10 +822,31 @@
       <c r="Z2" t="s">
         <v>46</v>
       </c>
+      <c r="AA2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
@@ -828,6 +922,27 @@
       </c>
       <c r="Z3" t="s">
         <v>46</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>